<commit_message>
Updated Database Model. Added missing foreign keys to the table "tblIterationData". (Tab "V2.0")
</commit_message>
<xml_diff>
--- a/Docs/Database Model.xlsx
+++ b/Docs/Database Model.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>Raw Data</t>
   </si>
@@ -173,7 +173,7 @@
     <t>speed</t>
   </si>
   <si>
-    <t>idCarriers</t>
+    <t>idCarrier</t>
   </si>
   <si>
     <t>accelaration</t>
@@ -198,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -225,7 +225,13 @@
       <color rgb="FF000000"/>
     </font>
     <font>
+      <color rgb="FF274E13"/>
+    </font>
+    <font>
       <color rgb="FF38761D"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -325,13 +331,16 @@
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -654,7 +663,7 @@
       <c r="A3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="17"/>
@@ -666,36 +675,36 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
+      <c r="B4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="20"/>
+      <c r="B5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21"/>
       <c r="D5" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="20"/>
+      <c r="B6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="21"/>
       <c r="D6" s="14" t="s">
         <v>46</v>
       </c>
@@ -710,7 +719,7 @@
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="18" t="s">
         <v>48</v>
       </c>
@@ -725,8 +734,8 @@
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
@@ -735,7 +744,7 @@
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="11" t="s">
         <v>51</v>
       </c>
@@ -748,7 +757,7 @@
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="14" t="s">
         <v>53</v>
       </c>
@@ -763,7 +772,7 @@
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="18" t="s">
         <v>55</v>
       </c>
@@ -778,11 +787,11 @@
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13">
-      <c r="C13" s="22"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14">
       <c r="A14" s="9" t="s">
@@ -790,7 +799,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
@@ -803,76 +812,106 @@
       <c r="D15" s="10"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
+      <c r="A18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24">
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26">
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27">
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>